<commit_message>
Updates Team Expense Split spreadsheet.
Updates the "Team_Expense_Split_Complete.xlsx" file.
The specific modifications are not discernible from the diff,
but this commit reflects a change to the binary file.
</commit_message>
<xml_diff>
--- a/Team_Expense_Split_Complete.xlsx
+++ b/Team_Expense_Split_Complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f4173669b36a6ab/Desktop/split-expense-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_BF99A0F5CC7D31FD0D61BD32054E1406DC8FA188" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C05F281-C1BA-4FDA-ABA1-12415F4E3DA9}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_BF99A0F5CC7D31FD0D61BD32054E1406DC8FA188" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A68075E1-1A42-420D-9C5F-3BD57B7AB5C1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>29.88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -478,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -486,7 +486,8 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>80</v>
+        <f>7.04+21.83</f>
+        <v>28.869999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -499,7 +500,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -718,11 +719,11 @@
       </c>
       <c r="B2">
         <f>'Shared Expenses'!B2</f>
-        <v>40</v>
+        <v>29.88</v>
       </c>
       <c r="C2">
         <f>SUM('Shared Expenses'!B2:B5)/4</f>
-        <v>75</v>
+        <v>14.6875</v>
       </c>
       <c r="D2">
         <f>SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!B2:B31, "Bergi")</f>
@@ -734,7 +735,7 @@
       </c>
       <c r="F2">
         <f>B2-C2-D2+E2</f>
-        <v>-35</v>
+        <v>15.192499999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -743,11 +744,11 @@
       </c>
       <c r="B3">
         <f>'Shared Expenses'!B3</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f>SUM('Shared Expenses'!B2:B5)/4</f>
-        <v>75</v>
+        <v>14.6875</v>
       </c>
       <c r="D3">
         <f>SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!B2:B31, "Nils")</f>
@@ -759,7 +760,7 @@
       </c>
       <c r="F3">
         <f>B3-C3-D3+E3</f>
-        <v>45</v>
+        <v>-14.6875</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -768,11 +769,11 @@
       </c>
       <c r="B4">
         <f>'Shared Expenses'!B4</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>SUM('Shared Expenses'!B2:B5)/4</f>
-        <v>75</v>
+        <v>14.6875</v>
       </c>
       <c r="D4">
         <f>SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!B2:B31, "Adrien")</f>
@@ -784,7 +785,7 @@
       </c>
       <c r="F4">
         <f>B4-C4-D4+E4</f>
-        <v>-15</v>
+        <v>-14.6875</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -793,11 +794,11 @@
       </c>
       <c r="B5">
         <f>'Shared Expenses'!B5</f>
-        <v>80</v>
+        <v>28.869999999999997</v>
       </c>
       <c r="C5">
         <f>SUM('Shared Expenses'!B2:B5)/4</f>
-        <v>75</v>
+        <v>14.6875</v>
       </c>
       <c r="D5">
         <f>SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!B2:B31, "Jason")</f>
@@ -809,7 +810,7 @@
       </c>
       <c r="F5">
         <f>B5-C5-D5+E5</f>
-        <v>5</v>
+        <v>14.182499999999997</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +846,7 @@
       </c>
       <c r="C2">
         <f>MAX(0, ('Shared Expenses'!B2 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Nils", 'Direct Expenses'!B2:B31, "Bergi"))</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <f>MAX(0, ('Shared Expenses'!B2 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Adrien", 'Direct Expenses'!B2:B31, "Bergi"))</f>
@@ -853,7 +854,7 @@
       </c>
       <c r="E2">
         <f>MAX(0, ('Shared Expenses'!B2 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B5 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Jason", 'Direct Expenses'!B2:B31, "Bergi"))</f>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -862,7 +863,7 @@
       </c>
       <c r="B3">
         <f>MAX(0, ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B2 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Bergi", 'Direct Expenses'!B2:B31, "Nils"))</f>
-        <v>0</v>
+        <v>14.6875</v>
       </c>
       <c r="D3">
         <f>MAX(0, ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Adrien", 'Direct Expenses'!B2:B31, "Nils"))</f>
@@ -870,7 +871,7 @@
       </c>
       <c r="E3">
         <f>MAX(0, ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B5 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Jason", 'Direct Expenses'!B2:B31, "Nils"))</f>
-        <v>0</v>
+        <v>14.6875</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -879,15 +880,15 @@
       </c>
       <c r="B4">
         <f>MAX(0, ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B2 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Bergi", 'Direct Expenses'!B2:B31, "Adrien"))</f>
-        <v>0</v>
+        <v>14.6875</v>
       </c>
       <c r="C4">
         <f>MAX(0, ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Nils", 'Direct Expenses'!B2:B31, "Adrien"))</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f>MAX(0, ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B5 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Jason", 'Direct Expenses'!B2:B31, "Adrien"))</f>
-        <v>15</v>
+        <v>14.6875</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
MOD : Update settlement recommendations
</commit_message>
<xml_diff>
--- a/Team_Expense_Split_Complete.xlsx
+++ b/Team_Expense_Split_Complete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f4173669b36a6ab/Desktop/split-expense-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_BF99A0F5CC7D31FD0D61BD32054E1406DC8FA188" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A68075E1-1A42-420D-9C5F-3BD57B7AB5C1}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_BF99A0F5CC7D31FD0D61BD32054E1406DC8FA188" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC522596-8B55-4D49-AAF1-496D24603CB7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19270" yWindow="10690" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shared Expenses" sheetId="1" r:id="rId1"/>
@@ -444,12 +444,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,15 +457,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>29.88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -473,15 +473,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -500,12 +500,12 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -519,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>0</v>
       </c>
@@ -527,7 +527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>0</v>
       </c>
@@ -535,142 +535,142 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>0</v>
       </c>
@@ -689,11 +689,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,17 +715,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <f>'Shared Expenses'!B2</f>
-        <v>29.88</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <f>SUM('Shared Expenses'!B2:B5)/4</f>
-        <v>14.6875</v>
+        <v>20.967500000000001</v>
       </c>
       <c r="D2">
         <f>SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!B2:B31, "Bergi")</f>
@@ -735,10 +737,10 @@
       </c>
       <c r="F2">
         <f>B2-C2-D2+E2</f>
-        <v>15.192499999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9.0324999999999989</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -748,7 +750,7 @@
       </c>
       <c r="C3">
         <f>SUM('Shared Expenses'!B2:B5)/4</f>
-        <v>14.6875</v>
+        <v>20.967500000000001</v>
       </c>
       <c r="D3">
         <f>SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!B2:B31, "Nils")</f>
@@ -760,20 +762,20 @@
       </c>
       <c r="F3">
         <f>B3-C3-D3+E3</f>
-        <v>-14.6875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>-20.967500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <f>'Shared Expenses'!B4</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <f>SUM('Shared Expenses'!B2:B5)/4</f>
-        <v>14.6875</v>
+        <v>20.967500000000001</v>
       </c>
       <c r="D4">
         <f>SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!B2:B31, "Adrien")</f>
@@ -785,10 +787,10 @@
       </c>
       <c r="F4">
         <f>B4-C4-D4+E4</f>
-        <v>-14.6875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4.0324999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -798,7 +800,7 @@
       </c>
       <c r="C5">
         <f>SUM('Shared Expenses'!B2:B5)/4</f>
-        <v>14.6875</v>
+        <v>20.967500000000001</v>
       </c>
       <c r="D5">
         <f>SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!B2:B31, "Jason")</f>
@@ -810,7 +812,7 @@
       </c>
       <c r="F5">
         <f>B5-C5-D5+E5</f>
-        <v>14.182499999999997</v>
+        <v>7.9024999999999963</v>
       </c>
     </row>
   </sheetData>
@@ -822,11 +824,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="B17:C22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -840,7 +844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -857,30 +861,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <f>MAX(0, ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B2 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Bergi", 'Direct Expenses'!B2:B31, "Nils"))</f>
-        <v>14.6875</v>
+        <v>20.967500000000001</v>
       </c>
       <c r="D3">
         <f>MAX(0, ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Adrien", 'Direct Expenses'!B2:B31, "Nils"))</f>
-        <v>0</v>
+        <v>20.967500000000001</v>
       </c>
       <c r="E3">
         <f>MAX(0, ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B5 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Jason", 'Direct Expenses'!B2:B31, "Nils"))</f>
-        <v>14.6875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20.967500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <f>MAX(0, ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B2 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Bergi", 'Direct Expenses'!B2:B31, "Adrien"))</f>
-        <v>14.6875</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>MAX(0, ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B3 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Nils", 'Direct Expenses'!B2:B31, "Adrien"))</f>
@@ -888,10 +892,10 @@
       </c>
       <c r="E4">
         <f>MAX(0, ('Shared Expenses'!B4 - SUM('Shared Expenses'!B2:B5)/4) * -1 * ('Shared Expenses'!B5 - SUM('Shared Expenses'!B2:B5)/4 &gt; 0)+SUMIFS('Direct Expenses'!C2:C31, 'Direct Expenses'!A2:A31, "Jason", 'Direct Expenses'!B2:B31, "Adrien"))</f>
-        <v>14.6875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -919,19 +923,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>

</xml_diff>